<commit_message>
finished psuedo code except edit system cant think how it is going to work! please look through and change what people think needs changing
</commit_message>
<xml_diff>
--- a/Pseudo Code/calculateResults.xlsx
+++ b/Pseudo Code/calculateResults.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Pseudo Code</t>
   </si>
@@ -65,9 +65,6 @@
     <t>WIN_POINTS int</t>
   </si>
   <si>
-    <t>DRAW_POINTS</t>
-  </si>
-  <si>
     <t>teamA</t>
   </si>
   <si>
@@ -132,6 +129,24 @@
   </si>
   <si>
     <t>END</t>
+  </si>
+  <si>
+    <t>\\home team always is team A</t>
+  </si>
+  <si>
+    <t>homeTeamID int</t>
+  </si>
+  <si>
+    <t>awayTeamID int</t>
+  </si>
+  <si>
+    <t>DRAW_POINTS int</t>
+  </si>
+  <si>
+    <t>teamBPoints = WIN_POINTS</t>
+  </si>
+  <si>
+    <t>teamAPoints = 0</t>
   </si>
 </sst>
 </file>
@@ -485,9 +500,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
@@ -495,9 +510,10 @@
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,80 +521,85 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C5" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
         <v>12</v>
@@ -587,7 +608,7 @@
     <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -609,28 +630,28 @@
     <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -647,100 +668,107 @@
     <row r="28" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B35" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B35" s="4" t="s">
+    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B36" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B36" s="4" t="s">
+    <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B37" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B37" s="4" t="s">
+    <row r="38" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B38" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B38" s="4" t="s">
+    <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B39" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B39" s="4" t="s">
+    <row r="40" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B40" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B41" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B42" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B43" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B45" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B46" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B40" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B41" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B42" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B43" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B44" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B45" s="4"/>
-    </row>
-    <row r="46" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B46" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>